<commit_message>
Post meeting update. Off des value correctly copied.
</commit_message>
<xml_diff>
--- a/Design.xlsx
+++ b/Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MSc 1\Q2\AE4263 - Modelling, Simulation and Application of Propulsion &amp; Power Systems\J57\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330AB08F-6C56-44F7-870E-B39796479898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB8346A-F340-48DC-B083-7C27F8FB62FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{0B3E99B5-5A71-4453-930C-E70929C225EA}"/>
   </bookViews>
@@ -85,7 +85,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -212,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -227,6 +227,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -236,16 +243,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4457,498 +4454,6 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>SFC</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> vs. Thrust</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Thrust</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Study!$C$2:$C$10</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>15621.948838117556</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20675.766760810326</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>34632.914198109509</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>45524.073129871074</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>46945.576383229192</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>54396.783191829178</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>61716.458133612017</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>67940.321221838734</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>73044.951863376715</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Study!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>25.605</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24.1829</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>21.6557</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>21.9664</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>22.085999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>22.979299999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24.3047</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>25.757899999999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>27.380400000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C64A-420B-AD35-5C7222F97F3F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="872189903"/>
-        <c:axId val="872188463"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="872189903"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="nl-NL"/>
-                  <a:t>Thrust [kN]</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="nl-NL"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="872188463"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="872188463"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="20"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="nl-NL"/>
-                  <a:t>SFC</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="nl-NL" baseline="0"/>
-                  <a:t> [g/kNs]</a:t>
-                </a:r>
-                <a:endParaRPr lang="nl-NL"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="nl-NL"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="872189903"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5760,46 +5265,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -9413,522 +8878,6 @@
 </file>
 
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -10719,16 +9668,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>154684</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>373759</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>113588</xdr:rowOff>
+      <xdr:rowOff>132638</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -10751,7 +9700,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5219700" y="3152775"/>
+          <a:off x="4829175" y="3171825"/>
           <a:ext cx="4078984" cy="2866313"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10805,51 +9754,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
+      <xdr:colOff>371475</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{888CA8A0-349E-5235-A797-4B9F98333A26}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10868,7 +9781,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -11211,18 +10124,18 @@
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="20"/>
+      <c r="F1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="13"/>
+      <c r="G1" s="20"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
@@ -11636,14 +10549,14 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="13" t="s">
+      <c r="B21" s="21"/>
+      <c r="C21" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="13"/>
+      <c r="D21" s="20"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
@@ -11691,7 +10604,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11700,18 +10613,18 @@
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="20"/>
+      <c r="F1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="13"/>
+      <c r="G1" s="20"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
@@ -11742,7 +10655,7 @@
       <c r="D3" s="3">
         <v>253.03</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="12">
         <v>253.03</v>
       </c>
       <c r="F3" s="2">
@@ -11765,13 +10678,13 @@
       <c r="D4" s="1">
         <v>253.03</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4">
         <v>253.03</v>
       </c>
       <c r="F4" s="1">
         <v>82.704999999999998</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4">
         <v>82.704999999999998</v>
       </c>
     </row>
@@ -11788,13 +10701,13 @@
       <c r="D5" s="1">
         <v>253.03</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5">
         <v>254.12</v>
       </c>
       <c r="F5" s="1">
         <v>82.704999999999998</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5">
         <v>83.962999999999994</v>
       </c>
     </row>
@@ -11811,13 +10724,13 @@
       <c r="D6" s="1">
         <v>401.05</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6">
         <v>400.35</v>
       </c>
       <c r="F6" s="1">
         <v>326.68400000000003</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6">
         <v>326.68400000000003</v>
       </c>
     </row>
@@ -11834,13 +10747,13 @@
       <c r="D7" s="1">
         <v>401.05</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7">
         <v>400.35</v>
       </c>
       <c r="F7" s="1">
         <v>320.15100000000001</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7">
         <v>320.15100000000001</v>
       </c>
     </row>
@@ -11857,13 +10770,13 @@
       <c r="D8" s="1">
         <v>598.4</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8">
         <v>597.11</v>
       </c>
       <c r="F8" s="1">
         <v>1120.528</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8">
         <v>1120.528</v>
       </c>
     </row>
@@ -11880,13 +10793,13 @@
       <c r="D9" s="1">
         <v>598.4</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9">
         <v>597.11</v>
       </c>
       <c r="F9" s="1">
         <v>1120.528</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9">
         <v>1120.528</v>
       </c>
     </row>
@@ -11903,13 +10816,13 @@
       <c r="D10" s="1">
         <v>1199</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10">
         <v>1189.3900000000001</v>
       </c>
       <c r="F10" s="1">
         <v>1058.8989999999999</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10">
         <v>1058.8989999999999</v>
       </c>
     </row>
@@ -11968,13 +10881,13 @@
       <c r="D14" s="1">
         <v>967.53</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14">
         <v>962.89</v>
       </c>
       <c r="F14" s="1">
         <v>462.38900000000001</v>
       </c>
-      <c r="G14" s="17">
+      <c r="G14">
         <v>458.17500000000001</v>
       </c>
     </row>
@@ -12005,13 +10918,13 @@
       <c r="D16" s="1">
         <v>831.49</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16">
         <v>828.62</v>
       </c>
       <c r="F16" s="1">
         <v>237.732</v>
       </c>
-      <c r="G16" s="17">
+      <c r="G16">
         <v>237.108</v>
       </c>
     </row>
@@ -12028,13 +10941,13 @@
       <c r="D17" s="1">
         <v>831.49</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17">
         <v>828.8</v>
       </c>
       <c r="F17" s="1">
         <v>227.16</v>
       </c>
-      <c r="G17" s="17">
+      <c r="G17">
         <v>226.53700000000001</v>
       </c>
     </row>
@@ -12051,25 +10964,25 @@
       <c r="D18" s="1">
         <v>831.49</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18">
         <v>638.37</v>
       </c>
       <c r="F18" s="1">
         <v>227.16</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18">
         <v>82.704999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="13" t="s">
+      <c r="B20" s="21"/>
+      <c r="C20" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="13"/>
+      <c r="D20" s="20"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
@@ -12095,7 +11008,7 @@
       <c r="C22">
         <v>22.1311</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="13">
         <v>22.226500000000001</v>
       </c>
     </row>
@@ -12117,7 +11030,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12126,18 +11039,18 @@
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="20"/>
+      <c r="F1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="13"/>
+      <c r="G1" s="20"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
@@ -12174,7 +11087,7 @@
       <c r="F3" s="3">
         <v>82.704999999999998</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3">
         <v>82.704999999999998</v>
       </c>
     </row>
@@ -12197,7 +11110,7 @@
       <c r="F4" s="1">
         <v>82.704999999999998</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4">
         <v>82.704999999999998</v>
       </c>
     </row>
@@ -12211,16 +11124,16 @@
       <c r="C5">
         <v>71.385000000000005</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="1">
         <v>254.12</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5">
         <v>254.12</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="1">
         <v>83.962999999999994</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5">
         <v>83.962000000000003</v>
       </c>
     </row>
@@ -12234,16 +11147,16 @@
       <c r="C6">
         <v>71.385000000000005</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="1">
         <v>400.35</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6">
         <v>399.54</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="1">
         <v>326.68400000000003</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6">
         <v>324.04700000000003</v>
       </c>
     </row>
@@ -12257,16 +11170,16 @@
       <c r="C7">
         <v>71.385000000000005</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="1">
         <v>400.35</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7">
         <v>399.54</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="1">
         <v>320.15100000000001</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7">
         <v>317.47500000000002</v>
       </c>
     </row>
@@ -12280,16 +11193,16 @@
       <c r="C8">
         <v>69.617000000000004</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="1">
         <v>597.11</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8">
         <v>601.44000000000005</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="1">
         <v>1120.528</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8">
         <v>1129.0050000000001</v>
       </c>
     </row>
@@ -12303,16 +11216,16 @@
       <c r="C9">
         <v>63.194000000000003</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="1">
         <v>597.11</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9">
         <v>601.44000000000005</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="1">
         <v>1120.528</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9">
         <v>1129.0050000000001</v>
       </c>
     </row>
@@ -12326,16 +11239,16 @@
       <c r="C10">
         <v>64.230999999999995</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="1">
         <v>1189.3900000000001</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10">
         <v>1189.83</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="1">
         <v>1058.8989999999999</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10">
         <v>1066.9090000000001</v>
       </c>
     </row>
@@ -12349,16 +11262,16 @@
       <c r="C11">
         <v>70.653999999999996</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="1">
         <v>962.89</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11">
         <v>960.12</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="1">
         <v>458.17500000000001</v>
       </c>
-      <c r="G11" s="17">
+      <c r="G11">
         <v>460.255</v>
       </c>
     </row>
@@ -12372,16 +11285,16 @@
       <c r="C12">
         <v>72.066999999999993</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="1">
         <v>828.62</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12">
         <v>825.33</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="1">
         <v>237.108</v>
       </c>
-      <c r="G12" s="17">
+      <c r="G12">
         <v>238.42500000000001</v>
       </c>
     </row>
@@ -12395,16 +11308,16 @@
       <c r="C13">
         <v>72.066999999999993</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="1">
         <v>828.8</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13">
         <v>825.51</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="1">
         <v>226.53700000000001</v>
       </c>
-      <c r="G13" s="17">
+      <c r="G13">
         <v>227.79</v>
       </c>
     </row>
@@ -12418,28 +11331,28 @@
       <c r="C14">
         <v>72.066999999999993</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="1">
         <v>638.37</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14">
         <v>634.77</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F14" s="1">
         <v>82.704999999999998</v>
       </c>
-      <c r="G14" s="17">
+      <c r="G14">
         <v>82.704999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="13" t="s">
+      <c r="B16" s="21"/>
+      <c r="C16" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="13"/>
+      <c r="D16" s="20"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -12459,10 +11372,10 @@
       <c r="A18" s="2">
         <v>46649</v>
       </c>
-      <c r="B18" s="16">
+      <c r="B18" s="12">
         <v>46946</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="13">
         <v>22.226500000000001</v>
       </c>
       <c r="D18">
@@ -12486,7 +11399,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12495,24 +11408,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="16" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="16">
+      <c r="A2" s="12">
         <v>0.4</v>
       </c>
       <c r="B2">
         <v>25.605</v>
       </c>
-      <c r="C2" s="23">
+      <c r="C2" s="17">
         <f>A2/B2*1000000</f>
         <v>15621.948838117556</v>
       </c>
@@ -12524,7 +11437,7 @@
       <c r="B3" s="1">
         <v>24.1829</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="18">
         <f t="shared" ref="C3:C10" si="0">A3/B3*1000000</f>
         <v>20675.766760810326</v>
       </c>
@@ -12536,7 +11449,7 @@
       <c r="B4" s="1">
         <v>21.6557</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="18">
         <f t="shared" si="0"/>
         <v>34632.914198109509</v>
       </c>
@@ -12548,7 +11461,7 @@
       <c r="B5" s="1">
         <v>21.9664</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="18">
         <f t="shared" si="0"/>
         <v>45524.073129871074</v>
       </c>
@@ -12560,7 +11473,7 @@
       <c r="B6" s="1">
         <v>22.085999999999999</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="18">
         <f t="shared" si="0"/>
         <v>46945.576383229192</v>
       </c>
@@ -12572,7 +11485,7 @@
       <c r="B7" s="1">
         <v>22.979299999999999</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="18">
         <f t="shared" si="0"/>
         <v>54396.783191829178</v>
       </c>
@@ -12584,7 +11497,7 @@
       <c r="B8" s="1">
         <v>24.3047</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="18">
         <f t="shared" si="0"/>
         <v>61716.458133612017</v>
       </c>
@@ -12596,7 +11509,7 @@
       <c r="B9" s="1">
         <v>25.757899999999999</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="18">
         <f t="shared" si="0"/>
         <v>67940.321221838734</v>
       </c>
@@ -12608,7 +11521,7 @@
       <c r="B10" s="1">
         <v>27.380400000000002</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="18">
         <f t="shared" si="0"/>
         <v>73044.951863376715</v>
       </c>

</xml_diff>

<commit_message>
Updates offdes / adp comparisson.
</commit_message>
<xml_diff>
--- a/Design.xlsx
+++ b/Design.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MSc 1\Q2\AE4263 - Modelling, Simulation and Application of Propulsion &amp; Power Systems\J57\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB8346A-F340-48DC-B083-7C27F8FB62FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BAD449-5AE2-4080-957B-4B8339103A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{0B3E99B5-5A71-4453-930C-E70929C225EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0B3E99B5-5A71-4453-930C-E70929C225EA}"/>
   </bookViews>
   <sheets>
     <sheet name="ADP_static" sheetId="1" r:id="rId1"/>
     <sheet name="ADP_dynamic" sheetId="3" r:id="rId2"/>
     <sheet name="OFFDES" sheetId="2" r:id="rId3"/>
-    <sheet name="Study" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="12">
   <si>
     <t>CRP</t>
   </si>
@@ -75,9 +74,6 @@
   </si>
   <si>
     <t>Thrust</t>
-  </si>
-  <si>
-    <t>Wfuel</t>
   </si>
 </sst>
 </file>
@@ -212,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -229,11 +225,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3964,987 +3955,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="nl-NL"/>
-              <a:t>SFC vs. Fuel</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="nl-NL" baseline="0"/>
-              <a:t> Flow</a:t>
-            </a:r>
-            <a:endParaRPr lang="nl-NL"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Study!$A$2:$A$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.03684</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.25</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.75</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Study!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>25.605</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24.1829</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>21.6557</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>21.9664</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>22.085999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>22.979299999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24.3047</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>25.757899999999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>27.380400000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FB3A-414D-9BA6-894C8A0A4FE8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="871787439"/>
-        <c:axId val="668048239"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="871787439"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="nl-NL"/>
-                  <a:t>Fuel</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="nl-NL" baseline="0"/>
-                  <a:t> Flow [kg/s]</a:t>
-                </a:r>
-                <a:endParaRPr lang="nl-NL"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="nl-NL"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="668048239"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="668048239"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="20"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="nl-NL"/>
-                  <a:t>SFC [g/kNs]</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="nl-NL"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="871787439"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>SFC</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> vs. Thrust</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Thrust</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Study!$C$2:$C$10</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>15621.948838117556</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20675.766760810326</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>34632.914198109509</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>45524.073129871074</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>46945.576383229192</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>54396.783191829178</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>61716.458133612017</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>67940.321221838734</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>73044.951863376715</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Study!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>25.605</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24.1829</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>21.6557</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>21.9664</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>22.085999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>22.979299999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24.3047</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>25.757899999999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>27.380400000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C64A-420B-AD35-5C7222F97F3F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="872189903"/>
-        <c:axId val="872188463"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="872189903"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="nl-NL"/>
-                  <a:t>Thrust [kN]</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="nl-NL"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="872188463"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="872188463"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="20"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="nl-NL"/>
-                  <a:t>SFC</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="nl-NL" baseline="0"/>
-                  <a:t> [g/kNs]</a:t>
-                </a:r>
-                <a:endParaRPr lang="nl-NL"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="nl-NL"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="872189903"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5185,86 +4195,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -7846,1038 +6776,6 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9713,83 +7611,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95EA396B-3085-5EA9-B5B4-BA7BCE08B3FD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B348DAE-E451-B695-67CB-00D790297423}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -10124,18 +7945,18 @@
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="20"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
@@ -10549,14 +8370,14 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="20" t="s">
+      <c r="B21" s="16"/>
+      <c r="C21" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="20"/>
+      <c r="D21" s="15"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
@@ -10603,8 +8424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8810E72B-BC27-4491-B736-1B8900857D53}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10613,18 +8434,18 @@
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="20"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
@@ -10975,14 +8796,14 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="20" t="s">
+      <c r="B20" s="16"/>
+      <c r="C20" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="20"/>
+      <c r="D20" s="15"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
@@ -11030,7 +8851,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11039,18 +8860,18 @@
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="20"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
@@ -11099,7 +8920,7 @@
         <v>70.953999999999994</v>
       </c>
       <c r="C4">
-        <v>71.385000000000005</v>
+        <v>71.461200000000005</v>
       </c>
       <c r="D4" s="1">
         <v>253.03</v>
@@ -11122,7 +8943,7 @@
         <v>70.953999999999994</v>
       </c>
       <c r="C5">
-        <v>71.385000000000005</v>
+        <v>71.461200000000005</v>
       </c>
       <c r="D5" s="1">
         <v>254.12</v>
@@ -11134,7 +8955,7 @@
         <v>83.962999999999994</v>
       </c>
       <c r="G5">
-        <v>83.962000000000003</v>
+        <v>83.962999999999994</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -11145,19 +8966,19 @@
         <v>70.953999999999994</v>
       </c>
       <c r="C6">
-        <v>71.385000000000005</v>
+        <v>71.461200000000005</v>
       </c>
       <c r="D6" s="1">
         <v>400.35</v>
       </c>
       <c r="E6">
-        <v>399.54</v>
+        <v>399.37</v>
       </c>
       <c r="F6" s="1">
         <v>326.68400000000003</v>
       </c>
       <c r="G6">
-        <v>324.04700000000003</v>
+        <v>323.38099999999997</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -11168,19 +8989,19 @@
         <v>70.953999999999994</v>
       </c>
       <c r="C7">
-        <v>71.385000000000005</v>
+        <v>71.461200000000005</v>
       </c>
       <c r="D7" s="1">
         <v>400.35</v>
       </c>
       <c r="E7">
-        <v>399.54</v>
+        <v>399.37</v>
       </c>
       <c r="F7" s="1">
         <v>320.15100000000001</v>
       </c>
       <c r="G7">
-        <v>317.47500000000002</v>
+        <v>316.80099999999999</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -11191,19 +9012,19 @@
         <v>69.194999999999993</v>
       </c>
       <c r="C8">
-        <v>69.617000000000004</v>
+        <v>69.691999999999993</v>
       </c>
       <c r="D8" s="1">
         <v>597.11</v>
       </c>
       <c r="E8">
-        <v>601.44000000000005</v>
+        <v>601.07000000000005</v>
       </c>
       <c r="F8" s="1">
         <v>1120.528</v>
       </c>
       <c r="G8">
-        <v>1129.0050000000001</v>
+        <v>1129.7439999999999</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -11214,19 +9035,19 @@
         <v>62.81</v>
       </c>
       <c r="C9">
-        <v>63.194000000000003</v>
+        <v>63.262</v>
       </c>
       <c r="D9" s="1">
         <v>597.11</v>
       </c>
       <c r="E9">
-        <v>601.44000000000005</v>
+        <v>601.07000000000005</v>
       </c>
       <c r="F9" s="1">
         <v>1120.528</v>
       </c>
       <c r="G9">
-        <v>1129.0050000000001</v>
+        <v>1129.7439999999999</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -11237,19 +9058,19 @@
         <v>63.847000000000001</v>
       </c>
       <c r="C10">
-        <v>64.230999999999995</v>
+        <v>64.299000000000007</v>
       </c>
       <c r="D10" s="1">
         <v>1189.3900000000001</v>
       </c>
       <c r="E10">
-        <v>1189.83</v>
+        <v>1188.93</v>
       </c>
       <c r="F10" s="1">
         <v>1058.8989999999999</v>
       </c>
       <c r="G10">
-        <v>1066.9090000000001</v>
+        <v>1067.6079999999999</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -11260,19 +9081,19 @@
         <v>70.23</v>
       </c>
       <c r="C11">
-        <v>70.653999999999996</v>
+        <v>70.728999999999999</v>
       </c>
       <c r="D11" s="1">
         <v>962.89</v>
       </c>
       <c r="E11">
-        <v>960.12</v>
+        <v>958.22</v>
       </c>
       <c r="F11" s="1">
         <v>458.17500000000001</v>
       </c>
       <c r="G11">
-        <v>460.255</v>
+        <v>460.572</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -11283,19 +9104,19 @@
         <v>71.635999999999996</v>
       </c>
       <c r="C12">
-        <v>72.066999999999993</v>
+        <v>72.143000000000001</v>
       </c>
       <c r="D12" s="1">
         <v>828.62</v>
       </c>
       <c r="E12">
-        <v>825.33</v>
+        <v>824.78</v>
       </c>
       <c r="F12" s="1">
         <v>237.108</v>
       </c>
       <c r="G12">
-        <v>238.42500000000001</v>
+        <v>238.66499999999999</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -11306,19 +9127,19 @@
         <v>71.635999999999996</v>
       </c>
       <c r="C13">
-        <v>72.066999999999993</v>
+        <v>72.143000000000001</v>
       </c>
       <c r="D13" s="1">
         <v>828.8</v>
       </c>
       <c r="E13">
-        <v>825.51</v>
+        <v>824.96</v>
       </c>
       <c r="F13" s="1">
         <v>226.53700000000001</v>
       </c>
       <c r="G13">
-        <v>227.79</v>
+        <v>228.018</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -11329,13 +9150,13 @@
         <v>71.635999999999996</v>
       </c>
       <c r="C14">
-        <v>72.066999999999993</v>
+        <v>72.143000000000001</v>
       </c>
       <c r="D14" s="1">
         <v>638.37</v>
       </c>
       <c r="E14">
-        <v>634.77</v>
+        <v>634.15</v>
       </c>
       <c r="F14" s="1">
         <v>82.704999999999998</v>
@@ -11345,14 +9166,14 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="20" t="s">
+      <c r="B16" s="16"/>
+      <c r="C16" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="20"/>
+      <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -11373,13 +9194,13 @@
         <v>46649</v>
       </c>
       <c r="B18" s="12">
-        <v>46946</v>
+        <v>43642</v>
       </c>
       <c r="C18" s="13">
         <v>22.226500000000001</v>
       </c>
       <c r="D18">
-        <v>22.085999999999999</v>
+        <v>22.061</v>
       </c>
     </row>
   </sheetData>
@@ -11392,142 +9213,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC18769F-C309-4F2C-B7F7-2AB0653FD583}">
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q29" sqref="Q29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
-        <v>0.4</v>
-      </c>
-      <c r="B2">
-        <v>25.605</v>
-      </c>
-      <c r="C2" s="17">
-        <f>A2/B2*1000000</f>
-        <v>15621.948838117556</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0.5</v>
-      </c>
-      <c r="B3" s="1">
-        <v>24.1829</v>
-      </c>
-      <c r="C3" s="18">
-        <f t="shared" ref="C3:C10" si="0">A3/B3*1000000</f>
-        <v>20675.766760810326</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0.75</v>
-      </c>
-      <c r="B4" s="1">
-        <v>21.6557</v>
-      </c>
-      <c r="C4" s="18">
-        <f t="shared" si="0"/>
-        <v>34632.914198109509</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1">
-        <v>21.9664</v>
-      </c>
-      <c r="C5" s="18">
-        <f t="shared" si="0"/>
-        <v>45524.073129871074</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1.03684</v>
-      </c>
-      <c r="B6" s="1">
-        <v>22.085999999999999</v>
-      </c>
-      <c r="C6" s="18">
-        <f t="shared" si="0"/>
-        <v>46945.576383229192</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1.25</v>
-      </c>
-      <c r="B7" s="1">
-        <v>22.979299999999999</v>
-      </c>
-      <c r="C7" s="18">
-        <f t="shared" si="0"/>
-        <v>54396.783191829178</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1.5</v>
-      </c>
-      <c r="B8" s="1">
-        <v>24.3047</v>
-      </c>
-      <c r="C8" s="18">
-        <f t="shared" si="0"/>
-        <v>61716.458133612017</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1.75</v>
-      </c>
-      <c r="B9" s="1">
-        <v>25.757899999999999</v>
-      </c>
-      <c r="C9" s="18">
-        <f t="shared" si="0"/>
-        <v>67940.321221838734</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1">
-        <v>27.380400000000002</v>
-      </c>
-      <c r="C10" s="18">
-        <f t="shared" si="0"/>
-        <v>73044.951863376715</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the values in excel sheet with off- and -on design sims
</commit_message>
<xml_diff>
--- a/Design.xlsx
+++ b/Design.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MSc 1\Q2\AE4263 - Modelling, Simulation and Application of Propulsion &amp; Power Systems\J57\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerbe\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BAD449-5AE2-4080-957B-4B8339103A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3186527-BB1F-4812-85E1-0DB252DB9C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0B3E99B5-5A71-4453-930C-E70929C225EA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="16200" firstSheet="3" activeTab="4" xr2:uid="{0B3E99B5-5A71-4453-930C-E70929C225EA}"/>
   </bookViews>
   <sheets>
     <sheet name="ADP_static" sheetId="1" r:id="rId1"/>
     <sheet name="ADP_dynamic" sheetId="3" r:id="rId2"/>
-    <sheet name="OFFDES" sheetId="2" r:id="rId3"/>
+    <sheet name="ADP_Nozzle_Included" sheetId="4" r:id="rId3"/>
+    <sheet name="OFFDES" sheetId="2" r:id="rId4"/>
+    <sheet name="OFFDES_Nozzle_Included" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="12">
   <si>
     <t>CRP</t>
   </si>
@@ -3955,6 +3957,1669 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Pressure</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>CRP</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ADP_Nozzle_Included!$H$4:$H$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ADP_Nozzle_Included!$F$4:$F$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>82.704999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82.704999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>326.68400000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>320.15100000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1120.528</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1120.528</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1058.8989999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1058.8989999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>462.38900000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>462.38900000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>462.38900000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>237.732</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>237.732</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>227.16</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>227.16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A628-4BEA-B3C8-F69E3AC1F36C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Model</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ADP_Nozzle_Included!$H$4:$H$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ADP_Nozzle_Included!$G$4:$G$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>82.704999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82.704999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>326.68400000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>320.15100000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1120.528</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1120.528</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1058.8989999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>458.03300000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>235.536</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>224.964</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>224.96433167642701</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-A628-4BEA-B3C8-F69E3AC1F36C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1649960784"/>
+        <c:axId val="1649936784"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1649960784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1649936784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1649936784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1649960784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Model</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ADP_Nozzle_Included!$H$4:$H$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ADP_Nozzle_Included!$E$4:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>253.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>253.03</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400.59</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400.59</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>597.45000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>597.45000000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1189.68</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>963.09</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>827.65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>827.65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>827.83574848179705</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-96FD-49B1-ABAE-097BEA1D2C03}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>CRP</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ADP_Nozzle_Included!$H$4:$H$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ADP_Nozzle_Included!$D$4:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>253.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>253.03</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>401.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>401.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>598.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>598.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1199</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1169.3399999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>985.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>967.53</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>967.53</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>836.52</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>831.49</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>831.49</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>831.49</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-96FD-49B1-ABAE-097BEA1D2C03}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1649968464"/>
+        <c:axId val="1649990544"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1649968464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1649990544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1649990544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1649968464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>CRP</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ADP_Nozzle_Included!$H$4:$H$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ADP_Nozzle_Included!$B$4:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>70.954999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70.954999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70.954999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70.954999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>69.748999999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>62.44</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>63.476999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>67.024000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>67.024000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>70.430000000000007</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>70.430000000000007</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70.430000000000007</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>71.635999999999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>71.635999999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>71.635999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1305-45AA-A19D-4DE7F9C6EE0F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Model</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ADP_Nozzle_Included!$H$4:$H$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ADP_Nozzle_Included!$C$4:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>70.953999999999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70.953999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70.953999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70.953999999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>69.19</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>62.81</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>63.85</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>70.23</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>71.635999999999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>71.635999999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>71.635999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1305-45AA-A19D-4DE7F9C6EE0F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1649987664"/>
+        <c:axId val="1649980944"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1649987664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1649980944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1649980944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1649987664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4195,6 +5860,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -6776,6 +8561,1554 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7611,6 +10944,163 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>206253</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>18037</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>161212</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02ACF61F-0AD3-4A04-B7F1-F3CCBDD65C4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4473453" y="3009899"/>
+          <a:ext cx="4078984" cy="2866313"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{739ACB16-1F72-5C26-C123-958C3D3FA424}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>595312</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>290512</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73FFC81F-E174-49B9-D2F1-9C34CE805A8C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>566737</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>261937</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E298152-63AF-D531-1D04-2A5BFDB8E620}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7931,7 +11421,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8424,8 +11914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8810E72B-BC27-4491-B736-1B8900857D53}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8847,11 +12337,502 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7577DE96-B984-4697-A938-32C3FE3543F6}">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="15"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3">
+        <v>253.03</v>
+      </c>
+      <c r="E3" s="2">
+        <v>253.03</v>
+      </c>
+      <c r="F3" s="3">
+        <v>82.704999999999998</v>
+      </c>
+      <c r="G3" s="2">
+        <v>82.704999999999998</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>70.954999999999998</v>
+      </c>
+      <c r="C4">
+        <v>70.953999999999994</v>
+      </c>
+      <c r="D4" s="1">
+        <v>253.03</v>
+      </c>
+      <c r="E4">
+        <v>253.03</v>
+      </c>
+      <c r="F4" s="1">
+        <v>82.704999999999998</v>
+      </c>
+      <c r="G4">
+        <v>82.704999999999998</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>70.954999999999998</v>
+      </c>
+      <c r="C5">
+        <v>70.953999999999994</v>
+      </c>
+      <c r="D5" s="1">
+        <v>253.03</v>
+      </c>
+      <c r="E5">
+        <v>253.03</v>
+      </c>
+      <c r="F5" s="1">
+        <v>82.704999999999998</v>
+      </c>
+      <c r="G5">
+        <v>82.704999999999998</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1">
+        <v>70.954999999999998</v>
+      </c>
+      <c r="C6">
+        <v>70.953999999999994</v>
+      </c>
+      <c r="D6" s="1">
+        <v>401.05</v>
+      </c>
+      <c r="E6">
+        <v>400.59</v>
+      </c>
+      <c r="F6" s="1">
+        <v>326.68400000000003</v>
+      </c>
+      <c r="G6">
+        <v>326.68400000000003</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1">
+        <v>70.954999999999998</v>
+      </c>
+      <c r="C7">
+        <v>70.953999999999994</v>
+      </c>
+      <c r="D7" s="1">
+        <v>401.05</v>
+      </c>
+      <c r="E7">
+        <v>400.59</v>
+      </c>
+      <c r="F7" s="1">
+        <v>320.15100000000001</v>
+      </c>
+      <c r="G7">
+        <v>320.15100000000001</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>69.748999999999995</v>
+      </c>
+      <c r="C8">
+        <v>69.19</v>
+      </c>
+      <c r="D8" s="1">
+        <v>598.4</v>
+      </c>
+      <c r="E8">
+        <v>597.45000000000005</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1120.528</v>
+      </c>
+      <c r="G8">
+        <v>1120.528</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1">
+        <v>62.44</v>
+      </c>
+      <c r="C9">
+        <v>62.81</v>
+      </c>
+      <c r="D9" s="1">
+        <v>598.4</v>
+      </c>
+      <c r="E9">
+        <v>597.45000000000005</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1120.528</v>
+      </c>
+      <c r="G9">
+        <v>1120.528</v>
+      </c>
+      <c r="H9">
+        <v>6</v>
+      </c>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1">
+        <v>63.476999999999997</v>
+      </c>
+      <c r="C10">
+        <v>63.85</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1199</v>
+      </c>
+      <c r="E10">
+        <v>1189.68</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1058.8989999999999</v>
+      </c>
+      <c r="G10">
+        <v>1058.8989999999999</v>
+      </c>
+      <c r="H10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>41</v>
+      </c>
+      <c r="B11" s="1">
+        <v>67.024000000000001</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1169.3399999999999</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1058.8989999999999</v>
+      </c>
+      <c r="H11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>43</v>
+      </c>
+      <c r="B12" s="1">
+        <v>67.024000000000001</v>
+      </c>
+      <c r="D12" s="1">
+        <v>985.25</v>
+      </c>
+      <c r="F12" s="1">
+        <v>462.38900000000001</v>
+      </c>
+      <c r="H12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>44</v>
+      </c>
+      <c r="B13" s="1">
+        <v>70.430000000000007</v>
+      </c>
+      <c r="D13" s="1">
+        <v>967.53</v>
+      </c>
+      <c r="F13" s="1">
+        <v>462.38900000000001</v>
+      </c>
+      <c r="H13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>45</v>
+      </c>
+      <c r="B14" s="1">
+        <v>70.430000000000007</v>
+      </c>
+      <c r="C14">
+        <v>70.23</v>
+      </c>
+      <c r="D14" s="1">
+        <v>967.53</v>
+      </c>
+      <c r="E14">
+        <v>963.09</v>
+      </c>
+      <c r="F14" s="1">
+        <v>462.38900000000001</v>
+      </c>
+      <c r="G14">
+        <v>458.03300000000002</v>
+      </c>
+      <c r="H14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>49</v>
+      </c>
+      <c r="B15" s="1">
+        <v>70.430000000000007</v>
+      </c>
+      <c r="D15" s="1">
+        <v>836.52</v>
+      </c>
+      <c r="F15" s="1">
+        <v>237.732</v>
+      </c>
+      <c r="H15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1">
+        <v>71.635999999999996</v>
+      </c>
+      <c r="C16">
+        <v>71.635999999999996</v>
+      </c>
+      <c r="D16" s="1">
+        <v>831.49</v>
+      </c>
+      <c r="E16">
+        <v>827.65</v>
+      </c>
+      <c r="F16" s="1">
+        <v>237.732</v>
+      </c>
+      <c r="G16">
+        <v>235.536</v>
+      </c>
+      <c r="H16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1">
+        <v>71.635999999999996</v>
+      </c>
+      <c r="C17">
+        <v>71.635999999999996</v>
+      </c>
+      <c r="D17" s="1">
+        <v>831.49</v>
+      </c>
+      <c r="E17">
+        <v>827.65</v>
+      </c>
+      <c r="F17" s="1">
+        <v>227.16</v>
+      </c>
+      <c r="G17">
+        <v>224.964</v>
+      </c>
+      <c r="H17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1">
+        <v>71.635999999999996</v>
+      </c>
+      <c r="C18">
+        <v>71.635999999999996</v>
+      </c>
+      <c r="D18" s="1">
+        <v>831.49</v>
+      </c>
+      <c r="E18">
+        <v>827.83574848179705</v>
+      </c>
+      <c r="F18" s="1">
+        <v>227.16</v>
+      </c>
+      <c r="G18">
+        <f>224964.331676427/1000</f>
+        <v>224.96433167642701</v>
+      </c>
+      <c r="H18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="D19" s="1">
+        <v>598.4</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1120.527</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="16"/>
+      <c r="C21" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="15"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>46850</v>
+      </c>
+      <c r="B23" s="7">
+        <v>46289.907518102002</v>
+      </c>
+      <c r="C23">
+        <v>22.1311</v>
+      </c>
+      <c r="D23">
+        <f>0.0000223988349856723*10^6</f>
+        <v>22.398834985672302</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B6162FC-271D-45A1-933D-2598E6077B4F}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9201,6 +13182,392 @@
       </c>
       <c r="D18">
         <v>22.061</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1BEA683-53EF-4A05-BC29-583B94D5FAB0}">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="15"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3">
+        <v>253.03</v>
+      </c>
+      <c r="E3">
+        <v>253.03</v>
+      </c>
+      <c r="F3" s="3">
+        <v>82.704999999999998</v>
+      </c>
+      <c r="G3">
+        <v>82.704999999999998</v>
+      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>70.953999999999994</v>
+      </c>
+      <c r="C4">
+        <v>71.448909285228794</v>
+      </c>
+      <c r="D4" s="1">
+        <v>253.03</v>
+      </c>
+      <c r="E4">
+        <v>253.03</v>
+      </c>
+      <c r="F4" s="1">
+        <v>82.704999999999998</v>
+      </c>
+      <c r="G4">
+        <v>82.704999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>70.953999999999994</v>
+      </c>
+      <c r="C5">
+        <v>71.448909285228794</v>
+      </c>
+      <c r="D5" s="1">
+        <v>253.03</v>
+      </c>
+      <c r="E5">
+        <v>253.03</v>
+      </c>
+      <c r="F5">
+        <v>82.704999999999998</v>
+      </c>
+      <c r="G5">
+        <v>82.704999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>70.953999999999994</v>
+      </c>
+      <c r="C6">
+        <v>71.448909285228794</v>
+      </c>
+      <c r="D6">
+        <v>400.59</v>
+      </c>
+      <c r="E6">
+        <v>398.648608638025</v>
+      </c>
+      <c r="F6" s="1">
+        <v>326.68400000000003</v>
+      </c>
+      <c r="G6">
+        <f>322823.169513018/1000</f>
+        <v>322.823169513018</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>70.953999999999994</v>
+      </c>
+      <c r="C7">
+        <v>71.448909285228794</v>
+      </c>
+      <c r="D7">
+        <v>400.59</v>
+      </c>
+      <c r="E7">
+        <v>398.648608638025</v>
+      </c>
+      <c r="F7" s="1">
+        <v>320.15100000000001</v>
+      </c>
+      <c r="G7">
+        <f>316244.601365199/1000</f>
+        <v>316.244601365199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>69.194999999999993</v>
+      </c>
+      <c r="C8">
+        <v>69.679804699355699</v>
+      </c>
+      <c r="D8">
+        <v>597.45000000000005</v>
+      </c>
+      <c r="E8">
+        <v>600.34058487631796</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1120.528</v>
+      </c>
+      <c r="G8">
+        <f>1129284.62391745/1000</f>
+        <v>1129.2846239174501</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>31</v>
+      </c>
+      <c r="B9">
+        <v>62.81</v>
+      </c>
+      <c r="C9">
+        <v>63.251033854477903</v>
+      </c>
+      <c r="D9">
+        <v>597.45000000000005</v>
+      </c>
+      <c r="E9">
+        <v>600.34058487631796</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1120.528</v>
+      </c>
+      <c r="G9">
+        <f>1129284.62391745/1000</f>
+        <v>1129.2846239174501</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>63.847000000000001</v>
+      </c>
+      <c r="C10">
+        <v>64.287708448777707</v>
+      </c>
+      <c r="D10">
+        <v>1189.68</v>
+      </c>
+      <c r="E10">
+        <v>1188.39903041047</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1058.8989999999999</v>
+      </c>
+      <c r="G10">
+        <f>1067173.96960199/1000</f>
+        <v>1067.1739696019899</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>45</v>
+      </c>
+      <c r="B11">
+        <v>70.23</v>
+      </c>
+      <c r="C11">
+        <v>70.716479293655397</v>
+      </c>
+      <c r="D11">
+        <v>963.09</v>
+      </c>
+      <c r="E11">
+        <v>957.68534393435596</v>
+      </c>
+      <c r="F11">
+        <v>458.03300000000002</v>
+      </c>
+      <c r="G11">
+        <f>460222.717181194/1000</f>
+        <v>460.22271718119401</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>71.635999999999996</v>
+      </c>
+      <c r="C12">
+        <v>72.130808879528601</v>
+      </c>
+      <c r="D12">
+        <v>827.65</v>
+      </c>
+      <c r="E12">
+        <v>822.72677454030804</v>
+      </c>
+      <c r="F12">
+        <v>235.536</v>
+      </c>
+      <c r="G12">
+        <f>236454.867737945/1000</f>
+        <v>236.45486773794499</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>71.635999999999996</v>
+      </c>
+      <c r="C13">
+        <v>72.130808879528601</v>
+      </c>
+      <c r="D13">
+        <v>827.65</v>
+      </c>
+      <c r="E13">
+        <v>822.90486988635098</v>
+      </c>
+      <c r="F13">
+        <v>224.964</v>
+      </c>
+      <c r="G13">
+        <v>225809.844125873</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>71.635999999999996</v>
+      </c>
+      <c r="C14">
+        <v>72.130808879528601</v>
+      </c>
+      <c r="D14">
+        <v>827.83574848179705</v>
+      </c>
+      <c r="E14">
+        <v>822.90486988635098</v>
+      </c>
+      <c r="F14">
+        <f>224964.331676427/1000</f>
+        <v>224.96433167642701</v>
+      </c>
+      <c r="G14">
+        <f>225809.844125873/1000</f>
+        <v>225.80984412587301</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="15"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>46289.907518102002</v>
+      </c>
+      <c r="B18" s="12">
+        <v>43642</v>
+      </c>
+      <c r="C18">
+        <f>0.0000223988349856723*10^6</f>
+        <v>22.398834985672302</v>
+      </c>
+      <c r="D18">
+        <f>0.0000222788675100606*10^6</f>
+        <v>22.2788675100606</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
scaled maps and made compressor maps for LHC and LPC
</commit_message>
<xml_diff>
--- a/Design.xlsx
+++ b/Design.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerbe\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boris\Documents\GitHub\AE4263-J57\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3186527-BB1F-4812-85E1-0DB252DB9C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9622D462-58C3-45B3-A510-CB62DE08C0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="16200" firstSheet="3" activeTab="4" xr2:uid="{0B3E99B5-5A71-4453-930C-E70929C225EA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{0B3E99B5-5A71-4453-930C-E70929C225EA}"/>
   </bookViews>
   <sheets>
     <sheet name="ADP_static" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="ADP_Nozzle_Included" sheetId="4" r:id="rId3"/>
     <sheet name="OFFDES" sheetId="2" r:id="rId4"/>
     <sheet name="OFFDES_Nozzle_Included" sheetId="5" r:id="rId5"/>
+    <sheet name="CASE_1" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="17">
   <si>
     <t>CRP</t>
   </si>
@@ -76,6 +77,21 @@
   </si>
   <si>
     <t>Thrust</t>
+  </si>
+  <si>
+    <t>LPC</t>
+  </si>
+  <si>
+    <t>HPC</t>
+  </si>
+  <si>
+    <t>Case 1</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Thurst Steps</t>
   </si>
 </sst>
 </file>
@@ -210,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -236,6 +252,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -862,6 +882,363 @@
         <a:defRPr/>
       </a:pPr>
       <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>SFC as function of </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-NL"/>
+              <a:t>T(net)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CASE_1!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SFC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>CASE_1!$B$3:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>21.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.646000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42.436</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46.707099999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>52.167999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>CASE_1!$C$3:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>24.594999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.74</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.268999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.199000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.427</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3BFD-4195-AF16-229F98097B4C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1595655104"/>
+        <c:axId val="1595657024"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1595655104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1595657024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1595657024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1595655104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5660,6 +6037,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5981,6 +6398,522 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -11101,6 +12034,197 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>594098</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>39283</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>289298</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>39283</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D96D8AB8-38D0-41F6-0348-F5252B1B14ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>78827</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>78827</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>525517</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>157643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0F6818C-8240-DAC7-7138-A39EEC3DA18A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7330965" y="4125310"/>
+          <a:ext cx="5281449" cy="3389574"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>18621</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>39414</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>525537</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>157655</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D68806E-5622-D976-9400-816D45242223}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7270759" y="223345"/>
+          <a:ext cx="5341675" cy="3429000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>453943</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>99984</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>206390</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>99391</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92B89CD5-0145-D968-6F33-D4E92905C5CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2292682" y="3562114"/>
+          <a:ext cx="4655751" cy="2914886"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -11424,14 +12548,14 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="0.140625" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="0.109375" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -11448,7 +12572,7 @@
       </c>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -11468,7 +12592,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -11490,7 +12614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -11516,7 +12640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -11542,7 +12666,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>24</v>
       </c>
@@ -11568,7 +12692,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>25</v>
       </c>
@@ -11594,7 +12718,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -11620,7 +12744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>31</v>
       </c>
@@ -11647,7 +12771,7 @@
       </c>
       <c r="I9" s="11"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>4</v>
       </c>
@@ -11673,7 +12797,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>41</v>
       </c>
@@ -11690,7 +12814,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>43</v>
       </c>
@@ -11707,7 +12831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>44</v>
       </c>
@@ -11724,7 +12848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>45</v>
       </c>
@@ -11750,7 +12874,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>49</v>
       </c>
@@ -11767,7 +12891,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>5</v>
       </c>
@@ -11793,7 +12917,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>6</v>
       </c>
@@ -11819,7 +12943,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>8</v>
       </c>
@@ -11845,7 +12969,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -11859,7 +12983,7 @@
         <v>1120.527</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>11</v>
       </c>
@@ -11869,7 +12993,7 @@
       </c>
       <c r="D21" s="15"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>0</v>
       </c>
@@ -11883,7 +13007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>46850</v>
       </c>
@@ -11915,12 +13039,12 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -11937,7 +13061,7 @@
       </c>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -11957,7 +13081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -11976,7 +13100,7 @@
         <v>82.704999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -11999,7 +13123,7 @@
         <v>82.704999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -12022,7 +13146,7 @@
         <v>83.962999999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>24</v>
       </c>
@@ -12045,7 +13169,7 @@
         <v>326.68400000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>25</v>
       </c>
@@ -12068,7 +13192,7 @@
         <v>320.15100000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -12091,7 +13215,7 @@
         <v>1120.528</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>31</v>
       </c>
@@ -12114,7 +13238,7 @@
         <v>1120.528</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>4</v>
       </c>
@@ -12137,7 +13261,7 @@
         <v>1058.8989999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>41</v>
       </c>
@@ -12151,7 +13275,7 @@
         <v>1058.8989999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>43</v>
       </c>
@@ -12165,7 +13289,7 @@
         <v>462.38900000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>44</v>
       </c>
@@ -12179,7 +13303,7 @@
         <v>462.38900000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>45</v>
       </c>
@@ -12202,7 +13326,7 @@
         <v>458.17500000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>49</v>
       </c>
@@ -12216,7 +13340,7 @@
         <v>237.732</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>5</v>
       </c>
@@ -12239,7 +13363,7 @@
         <v>237.108</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>6</v>
       </c>
@@ -12262,7 +13386,7 @@
         <v>226.53700000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>8</v>
       </c>
@@ -12285,7 +13409,7 @@
         <v>82.704999999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
         <v>11</v>
       </c>
@@ -12295,7 +13419,7 @@
       </c>
       <c r="D20" s="15"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>0</v>
       </c>
@@ -12309,7 +13433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>46850</v>
       </c>
@@ -12340,13 +13464,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7577DE96-B984-4697-A938-32C3FE3543F6}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView zoomScale="117" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -12363,7 +13487,7 @@
       </c>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -12383,7 +13507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -12405,7 +13529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -12431,7 +13555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -12457,7 +13581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>24</v>
       </c>
@@ -12483,7 +13607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>25</v>
       </c>
@@ -12509,7 +13633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -12535,7 +13659,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>31</v>
       </c>
@@ -12562,7 +13686,7 @@
       </c>
       <c r="I9" s="11"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>4</v>
       </c>
@@ -12588,7 +13712,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>41</v>
       </c>
@@ -12605,7 +13729,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>43</v>
       </c>
@@ -12622,7 +13746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>44</v>
       </c>
@@ -12639,7 +13763,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>45</v>
       </c>
@@ -12665,7 +13789,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>49</v>
       </c>
@@ -12682,7 +13806,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>5</v>
       </c>
@@ -12708,7 +13832,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>6</v>
       </c>
@@ -12734,7 +13858,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>8</v>
       </c>
@@ -12761,7 +13885,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -12775,7 +13899,7 @@
         <v>1120.527</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>11</v>
       </c>
@@ -12785,7 +13909,7 @@
       </c>
       <c r="D21" s="15"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>0</v>
       </c>
@@ -12799,7 +13923,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>46850</v>
       </c>
@@ -12832,12 +13956,12 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:G18"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -12854,7 +13978,7 @@
       </c>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
@@ -12874,7 +13998,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -12893,7 +14017,7 @@
         <v>82.704999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -12916,7 +14040,7 @@
         <v>82.704999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -12939,7 +14063,7 @@
         <v>83.962999999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>24</v>
       </c>
@@ -12962,7 +14086,7 @@
         <v>323.38099999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>25</v>
       </c>
@@ -12985,7 +14109,7 @@
         <v>316.80099999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>3</v>
       </c>
@@ -13008,7 +14132,7 @@
         <v>1129.7439999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>31</v>
       </c>
@@ -13031,7 +14155,7 @@
         <v>1129.7439999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>4</v>
       </c>
@@ -13054,7 +14178,7 @@
         <v>1067.6079999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>45</v>
       </c>
@@ -13077,7 +14201,7 @@
         <v>460.572</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>5</v>
       </c>
@@ -13100,7 +14224,7 @@
         <v>238.66499999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>6</v>
       </c>
@@ -13123,7 +14247,7 @@
         <v>228.018</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>8</v>
       </c>
@@ -13146,7 +14270,7 @@
         <v>82.704999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>11</v>
       </c>
@@ -13156,7 +14280,7 @@
       </c>
       <c r="D16" s="15"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>10</v>
       </c>
@@ -13170,7 +14294,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>46649</v>
       </c>
@@ -13200,13 +14324,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1BEA683-53EF-4A05-BC29-583B94D5FAB0}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -13223,7 +14347,7 @@
       </c>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
@@ -13243,7 +14367,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -13263,7 +14387,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -13286,7 +14410,7 @@
         <v>82.704999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -13309,7 +14433,7 @@
         <v>82.704999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>24</v>
       </c>
@@ -13333,7 +14457,7 @@
         <v>322.823169513018</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>25</v>
       </c>
@@ -13357,7 +14481,7 @@
         <v>316.244601365199</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>3</v>
       </c>
@@ -13381,7 +14505,7 @@
         <v>1129.2846239174501</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>31</v>
       </c>
@@ -13405,7 +14529,7 @@
         <v>1129.2846239174501</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>4</v>
       </c>
@@ -13429,7 +14553,7 @@
         <v>1067.1739696019899</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>45</v>
       </c>
@@ -13453,7 +14577,7 @@
         <v>460.22271718119401</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>5</v>
       </c>
@@ -13477,7 +14601,7 @@
         <v>236.45486773794499</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>6</v>
       </c>
@@ -13500,7 +14624,7 @@
         <v>225809.844125873</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>8</v>
       </c>
@@ -13525,12 +14649,12 @@
         <v>225.80984412587301</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="D15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>11</v>
       </c>
@@ -13540,7 +14664,7 @@
       </c>
       <c r="D16" s="15"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>10</v>
       </c>
@@ -13554,7 +14678,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>46289.907518102002</v>
       </c>
@@ -13580,4 +14704,109 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4532EA9-76CB-4C54-AA7E-3204518D88B5}">
+  <dimension ref="A1:T22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B3" s="12">
+        <v>21.75</v>
+      </c>
+      <c r="C3" s="2">
+        <v>24.594999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B4" s="7">
+        <v>28.646000000000001</v>
+      </c>
+      <c r="C4">
+        <v>23.74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B5" s="7">
+        <v>42.436</v>
+      </c>
+      <c r="C5">
+        <v>22.268999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B6" s="7">
+        <v>46.707099999999997</v>
+      </c>
+      <c r="C6">
+        <v>22.199000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B7" s="7">
+        <v>52.167999999999999</v>
+      </c>
+      <c r="C7">
+        <v>22.427</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B8" s="18"/>
+    </row>
+    <row r="19" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G19" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+    </row>
+    <row r="22" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="N22" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="N1:T1"/>
+    <mergeCell ref="N22:T22"/>
+    <mergeCell ref="G19:I19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>